<commit_message>
Handled floating point imprecision wrto threshold
</commit_message>
<xml_diff>
--- a/results/2012_reps_by_priority(1).xlsx
+++ b/results/2012_reps_by_priority(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/MM2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61B9861-C3E1-8248-8A60-6F0FA1ED8DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBC2987-3E95-5B43-BC5C-A62B8A892289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1000" windowWidth="26940" windowHeight="16440" xr2:uid="{498A944D-881C-2C4C-85C3-31154A405953}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="60">
   <si>
     <t>HOUSE SEAT</t>
   </si>
@@ -639,10 +639,10 @@
   <dimension ref="A1:U170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B161" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B139" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3:N170"/>
+      <selection pane="bottomRight" activeCell="V170" sqref="V170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11463,6 +11463,13 @@
         <v>0</v>
       </c>
       <c r="S169" s="5"/>
+      <c r="T169" t="s">
+        <v>12</v>
+      </c>
+      <c r="U169" t="str">
+        <f t="shared" ref="U169:U170" si="18">IF(T169&lt;&gt;J169,"DIFF", "SAME")</f>
+        <v>SAME</v>
+      </c>
     </row>
     <row r="170" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A170">
@@ -11520,6 +11527,13 @@
         <v>0</v>
       </c>
       <c r="S170" s="5"/>
+      <c r="T170" t="s">
+        <v>12</v>
+      </c>
+      <c r="U170" t="str">
+        <f t="shared" si="18"/>
+        <v>SAME</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>